<commit_message>
updating collection scripts to process collection data
</commit_message>
<xml_diff>
--- a/data/data_digitization/collection_data/field_note_data/1_raw_data/HJ-8-collection-entry.xlsx
+++ b/data/data_digitization/collection_data/field_note_data/1_raw_data/HJ-8-collection-entry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/collection_data/field_note_data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/collection_data/field_note_data/1_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71963BB6-3EF1-6D4D-928B-6E1CFC04F23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71852447-9F04-C841-8194-DCB9AB72C181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15320" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -2436,7 +2436,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2724,7 +2724,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2734,10 +2734,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="67" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomLeft" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>